<commit_message>
rescues mode and phonology md
</commit_message>
<xml_diff>
--- a/Ch_7_Sentence_Modes/Excel/Mode AND Nuc PA and Phonetics LMEMs.xlsx
+++ b/Ch_7_Sentence_Modes/Excel/Mode AND Nuc PA and Phonetics LMEMs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\antoi\Github\PhD\Ch_7_Sentence_Modes\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ABB49050-ACD9-4988-9364-6061221AF27E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0D8F94E-F1FD-43B2-A7AF-87CD73BBEA0C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" tabRatio="835" activeTab="5" xr2:uid="{5F934F14-35FB-48F8-B9CC-AA2F647F3C27}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" tabRatio="835" firstSheet="5" activeTab="8" xr2:uid="{5F934F14-35FB-48F8-B9CC-AA2F647F3C27}"/>
   </bookViews>
   <sheets>
     <sheet name="B0 Mode" sheetId="8" r:id="rId1"/>
@@ -5723,16 +5723,16 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FFE66101"/>
+      <color rgb="FFFF9F42"/>
+      <color rgb="FFB5B0F3"/>
       <color rgb="FF1B9E77"/>
-      <color rgb="FFE66101"/>
       <color rgb="FFFC8D62"/>
       <color rgb="FF7570B3"/>
       <color rgb="FFE7298A"/>
       <color rgb="FFD95F02"/>
       <color rgb="FFF2F2F2"/>
       <color rgb="FF66C2A5"/>
-      <color rgb="FFFFD92F"/>
-      <color rgb="FF8DA0CB"/>
     </mruColors>
   </colors>
   <extLst>
@@ -7934,7 +7934,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{89D9BBDE-F560-4823-9BAF-CE33F41188F5}" type="CELLRANGE">
+                    <a:fld id="{C91F21AA-7DBB-43BE-BD1C-062203AD38C5}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -7967,7 +7967,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{0AD738D4-9EF1-4ED8-8DBE-A2B3835BB958}" type="CELLRANGE">
+                    <a:fld id="{8FD6D409-1D31-4580-98AF-7A414D9E9130}" type="CELLRANGE">
                       <a:rPr lang="en-IE"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -8594,7 +8594,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{65A2D891-6568-4F75-A9C4-AFCFA2313CF7}" type="CELLRANGE">
+                    <a:fld id="{5EDF10E0-3C1A-4E26-861F-6B60C51871A7}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -8627,7 +8627,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{43C55299-F3A3-46F2-BD0A-CAB98C647DCE}" type="CELLRANGE">
+                    <a:fld id="{B21831EE-A9D2-4E7F-ACF8-713A1F19B871}" type="CELLRANGE">
                       <a:rPr lang="en-IE"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -8661,7 +8661,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{A52740A7-2D7B-4B0C-A9DB-074DF7F1C6E3}" type="CELLRANGE">
+                    <a:fld id="{05F69E1B-A523-425D-9C51-B6AA91E573ED}" type="CELLRANGE">
                       <a:rPr lang="en-IE"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -8695,7 +8695,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{4AA38390-644E-4AE7-8D20-E980E40AE695}" type="CELLRANGE">
+                    <a:fld id="{4DDCD7C6-18FA-4ED4-91B2-5127E787286D}" type="CELLRANGE">
                       <a:rPr lang="en-IE"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -9961,7 +9961,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{4A0D0E78-4937-4771-819C-E457398846F2}" type="CELLRANGE">
+                    <a:fld id="{DE8E5A7D-54FD-4A1E-A16D-B2F592E3D4AC}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -9994,7 +9994,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{DF9E6BB2-49F9-4BCA-9DDF-94C9A327447A}" type="CELLRANGE">
+                    <a:fld id="{1BDEEADA-BAF9-4AF1-9277-F03B0489C7EF}" type="CELLRANGE">
                       <a:rPr lang="en-IE"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -10028,7 +10028,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{DDF704CA-20F8-4EA6-B6D7-8D4ABBF70503}" type="CELLRANGE">
+                    <a:fld id="{89E849DF-4ED3-4350-BD99-ABD29328F294}" type="CELLRANGE">
                       <a:rPr lang="en-IE"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -10062,7 +10062,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{8039A577-93D8-4472-9BB3-2B3C4BBF5547}" type="CELLRANGE">
+                    <a:fld id="{7EF091AA-46F7-46F2-8624-F419CF842AA2}" type="CELLRANGE">
                       <a:rPr lang="en-IE"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -10738,7 +10738,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{FA2A84D0-93EE-4CFB-93B5-1840FFE3C1F8}" type="CELLRANGE">
+                    <a:fld id="{E5EB56EB-1393-448A-ABFA-8EC8BF6979D1}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -10771,7 +10771,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{366917D8-5F57-42B4-839B-E1AFC63A76FF}" type="CELLRANGE">
+                    <a:fld id="{FC63EF7F-0ABC-4B61-BD59-0B625B60C9A8}" type="CELLRANGE">
                       <a:rPr lang="en-IE"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -12495,84 +12495,15 @@
         <c:scatterStyle val="lineMarker"/>
         <c:varyColors val="0"/>
         <c:ser>
-          <c:idx val="1"/>
-          <c:order val="0"/>
+          <c:idx val="2"/>
+          <c:order val="1"/>
           <c:tx>
-            <c:strRef>
-              <c:f>'Graph Data'!$A$3</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>MDC</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
+            <c:v> a. % H* L* L*H %</c:v>
           </c:tx>
           <c:spPr>
             <a:ln w="38100">
               <a:solidFill>
-                <a:srgbClr val="7570B3"/>
-              </a:solidFill>
-            </a:ln>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
-          <c:xVal>
-            <c:numRef>
-              <c:f>('Graph Data'!$B$3,'Graph Data'!$B$14)</c:f>
-              <c:numCache>
-                <c:formatCode>0</c:formatCode>
-                <c:ptCount val="2"/>
-                <c:pt idx="0">
-                  <c:v>94.498000000000005</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>318.06299999999999</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:xVal>
-          <c:yVal>
-            <c:numRef>
-              <c:f>('Graph Data'!$K$3,'Graph Data'!$K$14)</c:f>
-              <c:numCache>
-                <c:formatCode>0.0</c:formatCode>
-                <c:ptCount val="2"/>
-                <c:pt idx="0">
-                  <c:v>86.834999999999994</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>92.555000000000007</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:yVal>
-          <c:smooth val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-FADB-4C93-A067-1456C06C53AF}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="2"/>
-          <c:order val="1"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>'Graph Data'!$A$4</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>MWH</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="38100">
-              <a:solidFill>
-                <a:srgbClr val="FC8D62"/>
+                <a:srgbClr val="E66101"/>
               </a:solidFill>
             </a:ln>
           </c:spPr>
@@ -12617,124 +12548,34 @@
           </c:extLst>
         </c:ser>
         <c:ser>
-          <c:idx val="3"/>
-          <c:order val="2"/>
+          <c:idx val="4"/>
+          <c:order val="4"/>
           <c:tx>
-            <c:strRef>
-              <c:f>'Graph Data'!$A$5</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>MYN</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
+            <c:v> b. % H* !H* L*H %</c:v>
           </c:tx>
           <c:spPr>
             <a:ln w="38100">
               <a:solidFill>
-                <a:srgbClr val="1B9E77"/>
+                <a:srgbClr val="FF9F42"/>
               </a:solidFill>
             </a:ln>
           </c:spPr>
           <c:marker>
             <c:symbol val="none"/>
           </c:marker>
-          <c:xVal>
-            <c:numRef>
-              <c:f>('Graph Data'!$B$5,'Graph Data'!$B$16)</c:f>
-              <c:numCache>
-                <c:formatCode>0</c:formatCode>
-                <c:ptCount val="2"/>
-                <c:pt idx="0">
-                  <c:v>96.585999999999999</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>317.72000000000003</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:xVal>
           <c:yVal>
-            <c:numRef>
-              <c:f>('Graph Data'!$K$5,'Graph Data'!$K$16)</c:f>
-              <c:numCache>
-                <c:formatCode>0.0</c:formatCode>
-                <c:ptCount val="2"/>
-                <c:pt idx="0">
-                  <c:v>87.975999999999999</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>93.634</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
+            <c:numLit>
+              <c:formatCode>General</c:formatCode>
+              <c:ptCount val="1"/>
+              <c:pt idx="0">
+                <c:v>1</c:v>
+              </c:pt>
+            </c:numLit>
           </c:yVal>
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000002-FADB-4C93-A067-1456C06C53AF}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="0"/>
-          <c:order val="3"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>'Graph Data'!$A$6</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>MDQ</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="38100">
-              <a:solidFill>
-                <a:srgbClr val="E7298A"/>
-              </a:solidFill>
-            </a:ln>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
-          <c:xVal>
-            <c:numRef>
-              <c:f>('Graph Data'!$B$6,'Graph Data'!$B$17)</c:f>
-              <c:numCache>
-                <c:formatCode>0</c:formatCode>
-                <c:ptCount val="2"/>
-                <c:pt idx="0">
-                  <c:v>79.626999999999995</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>303.755</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:xVal>
-          <c:yVal>
-            <c:numRef>
-              <c:f>('Graph Data'!$K$6,'Graph Data'!$K$17)</c:f>
-              <c:numCache>
-                <c:formatCode>0.0</c:formatCode>
-                <c:ptCount val="2"/>
-                <c:pt idx="0">
-                  <c:v>87.183000000000007</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>94.043000000000006</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:yVal>
-          <c:smooth val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000003-FADB-4C93-A067-1456C06C53AF}"/>
+              <c16:uniqueId val="{00000000-A164-4DA6-AD07-82E406823E2D}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -12748,11 +12589,217 @@
         </c:dLbls>
         <c:axId val="950869344"/>
         <c:axId val="765174752"/>
+        <c:extLst>
+          <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+            <c15:filteredScatterSeries>
+              <c15:ser>
+                <c:idx val="1"/>
+                <c:order val="0"/>
+                <c:tx>
+                  <c:v> a. % H* L* L*H %</c:v>
+                </c:tx>
+                <c:spPr>
+                  <a:ln w="38100">
+                    <a:solidFill>
+                      <a:srgbClr val="7570B3"/>
+                    </a:solidFill>
+                  </a:ln>
+                </c:spPr>
+                <c:marker>
+                  <c:symbol val="none"/>
+                </c:marker>
+                <c:xVal>
+                  <c:numRef>
+                    <c:extLst>
+                      <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>('Graph Data'!$B$3,'Graph Data'!$B$14)</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:numCache>
+                      <c:formatCode>0</c:formatCode>
+                      <c:ptCount val="2"/>
+                      <c:pt idx="0">
+                        <c:v>94.498000000000005</c:v>
+                      </c:pt>
+                      <c:pt idx="1">
+                        <c:v>318.06299999999999</c:v>
+                      </c:pt>
+                    </c:numCache>
+                  </c:numRef>
+                </c:xVal>
+                <c:yVal>
+                  <c:numRef>
+                    <c:extLst>
+                      <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>('Graph Data'!$K$3,'Graph Data'!$K$14)</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:numCache>
+                      <c:formatCode>0.0</c:formatCode>
+                      <c:ptCount val="2"/>
+                      <c:pt idx="0">
+                        <c:v>86.834999999999994</c:v>
+                      </c:pt>
+                      <c:pt idx="1">
+                        <c:v>92.555000000000007</c:v>
+                      </c:pt>
+                    </c:numCache>
+                  </c:numRef>
+                </c:yVal>
+                <c:smooth val="0"/>
+                <c:extLst>
+                  <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                    <c16:uniqueId val="{00000000-FADB-4C93-A067-1456C06C53AF}"/>
+                  </c:ext>
+                </c:extLst>
+              </c15:ser>
+            </c15:filteredScatterSeries>
+            <c15:filteredScatterSeries>
+              <c15:ser>
+                <c:idx val="3"/>
+                <c:order val="2"/>
+                <c:tx>
+                  <c:v> c. %H (*) L*H %</c:v>
+                </c:tx>
+                <c:spPr>
+                  <a:ln w="38100">
+                    <a:solidFill>
+                      <a:srgbClr val="1B9E77"/>
+                    </a:solidFill>
+                  </a:ln>
+                </c:spPr>
+                <c:marker>
+                  <c:symbol val="none"/>
+                </c:marker>
+                <c:xVal>
+                  <c:numRef>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
+                      <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>('Graph Data'!$B$5,'Graph Data'!$B$16)</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:numCache>
+                      <c:formatCode>0</c:formatCode>
+                      <c:ptCount val="2"/>
+                      <c:pt idx="0">
+                        <c:v>96.585999999999999</c:v>
+                      </c:pt>
+                      <c:pt idx="1">
+                        <c:v>317.72000000000003</c:v>
+                      </c:pt>
+                    </c:numCache>
+                  </c:numRef>
+                </c:xVal>
+                <c:yVal>
+                  <c:numRef>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
+                      <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>('Graph Data'!$K$5,'Graph Data'!$K$16)</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:numCache>
+                      <c:formatCode>0.0</c:formatCode>
+                      <c:ptCount val="2"/>
+                      <c:pt idx="0">
+                        <c:v>87.975999999999999</c:v>
+                      </c:pt>
+                      <c:pt idx="1">
+                        <c:v>93.634</c:v>
+                      </c:pt>
+                    </c:numCache>
+                  </c:numRef>
+                </c:yVal>
+                <c:smooth val="0"/>
+                <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
+                  <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                    <c16:uniqueId val="{00000002-FADB-4C93-A067-1456C06C53AF}"/>
+                  </c:ext>
+                </c:extLst>
+              </c15:ser>
+            </c15:filteredScatterSeries>
+            <c15:filteredScatterSeries>
+              <c15:ser>
+                <c:idx val="0"/>
+                <c:order val="3"/>
+                <c:tx>
+                  <c:v> d. % H* (*) L*H %</c:v>
+                </c:tx>
+                <c:spPr>
+                  <a:ln w="38100">
+                    <a:solidFill>
+                      <a:srgbClr val="B5B0F3"/>
+                    </a:solidFill>
+                  </a:ln>
+                </c:spPr>
+                <c:marker>
+                  <c:symbol val="none"/>
+                </c:marker>
+                <c:xVal>
+                  <c:numRef>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
+                      <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>('Graph Data'!$B$6,'Graph Data'!$B$17)</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:numCache>
+                      <c:formatCode>0</c:formatCode>
+                      <c:ptCount val="2"/>
+                      <c:pt idx="0">
+                        <c:v>79.626999999999995</c:v>
+                      </c:pt>
+                      <c:pt idx="1">
+                        <c:v>303.755</c:v>
+                      </c:pt>
+                    </c:numCache>
+                  </c:numRef>
+                </c:xVal>
+                <c:yVal>
+                  <c:numRef>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
+                      <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>('Graph Data'!$K$6,'Graph Data'!$K$17)</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:numCache>
+                      <c:formatCode>0.0</c:formatCode>
+                      <c:ptCount val="2"/>
+                      <c:pt idx="0">
+                        <c:v>87.183000000000007</c:v>
+                      </c:pt>
+                      <c:pt idx="1">
+                        <c:v>94.043000000000006</c:v>
+                      </c:pt>
+                    </c:numCache>
+                  </c:numRef>
+                </c:yVal>
+                <c:smooth val="0"/>
+                <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
+                  <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                    <c16:uniqueId val="{00000003-FADB-4C93-A067-1456C06C53AF}"/>
+                  </c:ext>
+                </c:extLst>
+              </c15:ser>
+            </c15:filteredScatterSeries>
+          </c:ext>
+        </c:extLst>
       </c:scatterChart>
       <c:valAx>
         <c:axId val="950869344"/>
         <c:scaling>
           <c:orientation val="minMax"/>
+          <c:max val="600"/>
           <c:min val="0"/>
         </c:scaling>
         <c:delete val="0"/>
@@ -12932,10 +12979,10 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.65730375439286615"/>
-          <c:y val="0.52522304072404857"/>
-          <c:w val="0.25228480891784705"/>
-          <c:h val="0.2537818862825918"/>
+          <c:x val="0.66137719198143707"/>
+          <c:y val="0.24909829825297367"/>
+          <c:w val="0.27489919738293583"/>
+          <c:h val="0.16143492169609111"/>
         </c:manualLayout>
       </c:layout>
       <c:overlay val="1"/>
@@ -12944,11 +12991,7 @@
           <a:schemeClr val="bg1"/>
         </a:solidFill>
         <a:ln>
-          <a:solidFill>
-            <a:schemeClr val="bg2">
-              <a:lumMod val="90000"/>
-            </a:schemeClr>
-          </a:solidFill>
+          <a:noFill/>
         </a:ln>
       </c:spPr>
       <c:txPr>
@@ -25688,8 +25731,8 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>256310</xdr:colOff>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>381000</xdr:colOff>
       <xdr:row>14</xdr:row>
       <xdr:rowOff>153310</xdr:rowOff>
     </xdr:to>
@@ -42560,7 +42603,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E6DF4A6B-607B-48B2-B587-59CE43E9BBC5}">
   <dimension ref="G5:AB33"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="T19" sqref="T19"/>
     </sheetView>
   </sheetViews>
@@ -42595,7 +42638,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5FA75D8A-458C-4EF4-8CA5-966D1B6FEE89}">
   <dimension ref="A1:AC60"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A4" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView showGridLines="0" topLeftCell="A3" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="E25" sqref="E25"/>
     </sheetView>
   </sheetViews>
@@ -46128,14 +46171,69 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F5919AE2-0160-41E7-B7DF-2FBBFC2636AC}">
-  <dimension ref="A1"/>
+  <dimension ref="K17:L25"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I5" sqref="I5"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I3" sqref="I3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData/>
+  <sheetData>
+    <row r="17" spans="11:12" x14ac:dyDescent="0.3">
+      <c r="K17">
+        <v>0.85098039199999997</v>
+      </c>
+      <c r="L17" t="str">
+        <f>DEC2HEX((ROUND(K17*255,0)))</f>
+        <v>D9</v>
+      </c>
+    </row>
+    <row r="18" spans="11:12" x14ac:dyDescent="0.3">
+      <c r="K18">
+        <v>0.37254902000000001</v>
+      </c>
+      <c r="L18" t="str">
+        <f t="shared" ref="L18:L19" si="0">DEC2HEX((ROUND(K18*255,0)))</f>
+        <v>5F</v>
+      </c>
+    </row>
+    <row r="19" spans="11:12" x14ac:dyDescent="0.3">
+      <c r="K19">
+        <v>7.843137E-3</v>
+      </c>
+      <c r="L19" t="str">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="23" spans="11:12" x14ac:dyDescent="0.3">
+      <c r="K23">
+        <v>1</v>
+      </c>
+      <c r="L23" t="str">
+        <f t="shared" ref="L23:L25" si="1">DEC2HEX((ROUND(K23*255,0)))</f>
+        <v>FF</v>
+      </c>
+    </row>
+    <row r="24" spans="11:12" x14ac:dyDescent="0.3">
+      <c r="K24">
+        <v>0.62254902000000001</v>
+      </c>
+      <c r="L24" t="str">
+        <f t="shared" si="1"/>
+        <v>9F</v>
+      </c>
+    </row>
+    <row r="25" spans="11:12" x14ac:dyDescent="0.3">
+      <c r="K25">
+        <v>0.257843137</v>
+      </c>
+      <c r="L25" t="str">
+        <f t="shared" si="1"/>
+        <v>42</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
correcting p and improving phono analysis
</commit_message>
<xml_diff>
--- a/Ch_7_Sentence_Modes/Excel/Mode AND Nuc PA and Phonetics LMEMs.xlsx
+++ b/Ch_7_Sentence_Modes/Excel/Mode AND Nuc PA and Phonetics LMEMs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\antoi\Github\PhD\Ch_7_Sentence_Modes\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0D8F94E-F1FD-43B2-A7AF-87CD73BBEA0C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A57DA34B-01B2-4AE4-A584-A60505695F6C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" tabRatio="835" firstSheet="5" activeTab="8" xr2:uid="{5F934F14-35FB-48F8-B9CC-AA2F647F3C27}"/>
   </bookViews>
@@ -7934,7 +7934,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{C91F21AA-7DBB-43BE-BD1C-062203AD38C5}" type="CELLRANGE">
+                    <a:fld id="{DCEB0A6D-7155-4813-968D-AFB92A3A81DD}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -7967,7 +7967,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{8FD6D409-1D31-4580-98AF-7A414D9E9130}" type="CELLRANGE">
+                    <a:fld id="{F5910CB5-FF10-43DD-8684-53AE797AFB0B}" type="CELLRANGE">
                       <a:rPr lang="en-IE"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -8594,7 +8594,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{5EDF10E0-3C1A-4E26-861F-6B60C51871A7}" type="CELLRANGE">
+                    <a:fld id="{873C750E-617F-4C40-B9EB-7FE220576FAB}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -8627,7 +8627,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{B21831EE-A9D2-4E7F-ACF8-713A1F19B871}" type="CELLRANGE">
+                    <a:fld id="{382CDCC6-C650-4EBF-9963-7909B3EE574D}" type="CELLRANGE">
                       <a:rPr lang="en-IE"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -8661,7 +8661,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{05F69E1B-A523-425D-9C51-B6AA91E573ED}" type="CELLRANGE">
+                    <a:fld id="{3AC344D8-5F0B-47C0-BAC8-42993DAF5222}" type="CELLRANGE">
                       <a:rPr lang="en-IE"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -8695,7 +8695,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{4DDCD7C6-18FA-4ED4-91B2-5127E787286D}" type="CELLRANGE">
+                    <a:fld id="{3198F9B6-6EB9-4522-8713-01570D9ACF58}" type="CELLRANGE">
                       <a:rPr lang="en-IE"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -9345,7 +9345,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{208BAFFF-011F-433C-BD6A-217BAA6C4C16}" type="CELLRANGE">
+                    <a:fld id="{367CFE36-DE18-4584-839A-D904C711BA4B}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -9961,7 +9961,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{DE8E5A7D-54FD-4A1E-A16D-B2F592E3D4AC}" type="CELLRANGE">
+                    <a:fld id="{ED5F9C26-996E-4231-9AB3-7DC419DABAAE}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -9994,7 +9994,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{1BDEEADA-BAF9-4AF1-9277-F03B0489C7EF}" type="CELLRANGE">
+                    <a:fld id="{3D1009CD-CEE6-46B4-9B4E-A0B637DBBE36}" type="CELLRANGE">
                       <a:rPr lang="en-IE"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -10028,7 +10028,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{89E849DF-4ED3-4350-BD99-ABD29328F294}" type="CELLRANGE">
+                    <a:fld id="{FEB67ECB-8B75-4FF3-83FF-9CD1B35F20D7}" type="CELLRANGE">
                       <a:rPr lang="en-IE"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -10062,7 +10062,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{7EF091AA-46F7-46F2-8624-F419CF842AA2}" type="CELLRANGE">
+                    <a:fld id="{49180862-E6D4-4150-A6C4-F7300634ED95}" type="CELLRANGE">
                       <a:rPr lang="en-IE"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -10738,7 +10738,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{E5EB56EB-1393-448A-ABFA-8EC8BF6979D1}" type="CELLRANGE">
+                    <a:fld id="{886098FA-939F-42B7-AC79-ED3A8B604200}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -10771,7 +10771,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{FC63EF7F-0ABC-4B61-BD59-0B625B60C9A8}" type="CELLRANGE">
+                    <a:fld id="{C9D041ED-D856-4C17-99C4-15A60D09E8E9}" type="CELLRANGE">
                       <a:rPr lang="en-IE"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -11376,7 +11376,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{CB8E66F0-3445-4478-8E42-61CF3B337711}" type="CELLRANGE">
+                    <a:fld id="{378B9147-7CAB-4824-B192-3FE42688A85D}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -12496,9 +12496,9 @@
         <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="2"/>
-          <c:order val="1"/>
+          <c:order val="0"/>
           <c:tx>
-            <c:v> a. % H* L* L*H %</c:v>
+            <c:v> a. % H* L* H L*H %</c:v>
           </c:tx>
           <c:spPr>
             <a:ln w="38100">
@@ -12548,10 +12548,10 @@
           </c:extLst>
         </c:ser>
         <c:ser>
-          <c:idx val="4"/>
-          <c:order val="4"/>
+          <c:idx val="0"/>
+          <c:order val="3"/>
           <c:tx>
-            <c:v> b. % H* !H* L*H %</c:v>
+            <c:v> b. % H* L*!H L*H %</c:v>
           </c:tx>
           <c:spPr>
             <a:ln w="38100">
@@ -12563,19 +12563,97 @@
           <c:marker>
             <c:symbol val="none"/>
           </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>('Graph Data'!$B$6,'Graph Data'!$B$17)</c:f>
+              <c:numCache>
+                <c:formatCode>0</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>79.626999999999995</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>303.755</c:v>
+                </c:pt>
+              </c:numCache>
+              <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart"/>
+            </c:numRef>
+          </c:xVal>
           <c:yVal>
-            <c:numLit>
-              <c:formatCode>General</c:formatCode>
-              <c:ptCount val="1"/>
-              <c:pt idx="0">
-                <c:v>1</c:v>
-              </c:pt>
-            </c:numLit>
+            <c:numRef>
+              <c:f>('Graph Data'!$K$6,'Graph Data'!$K$17)</c:f>
+              <c:numCache>
+                <c:formatCode>0.0</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>87.183000000000007</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>94.043000000000006</c:v>
+                </c:pt>
+              </c:numCache>
+              <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart"/>
+            </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
-          <c:extLst>
+          <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-A164-4DA6-AD07-82E406823E2D}"/>
+              <c16:uniqueId val="{00000003-FADB-4C93-A067-1456C06C53AF}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="4"/>
+          <c:tx>
+            <c:v> c. % H* L* L*H %</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="38100">
+              <a:solidFill>
+                <a:srgbClr val="7570B3"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>('Graph Data'!$B$3,'Graph Data'!$B$14)</c:f>
+              <c:numCache>
+                <c:formatCode>0</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>94.498000000000005</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>318.06299999999999</c:v>
+                </c:pt>
+              </c:numCache>
+              <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart"/>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>('Graph Data'!$K$3,'Graph Data'!$K$14)</c:f>
+              <c:numCache>
+                <c:formatCode>0.0</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>86.834999999999994</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>92.555000000000007</c:v>
+                </c:pt>
+              </c:numCache>
+              <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart"/>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-FADB-4C93-A067-1456C06C53AF}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -12593,67 +12671,27 @@
           <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
             <c15:filteredScatterSeries>
               <c15:ser>
-                <c:idx val="1"/>
-                <c:order val="0"/>
+                <c:idx val="4"/>
+                <c:order val="1"/>
                 <c:tx>
-                  <c:v> a. % H* L* L*H %</c:v>
+                  <c:v> b. % H* L*!H L*H %</c:v>
                 </c:tx>
-                <c:spPr>
-                  <a:ln w="38100">
-                    <a:solidFill>
-                      <a:srgbClr val="7570B3"/>
-                    </a:solidFill>
-                  </a:ln>
-                </c:spPr>
                 <c:marker>
                   <c:symbol val="none"/>
                 </c:marker>
-                <c:xVal>
-                  <c:numRef>
-                    <c:extLst>
-                      <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
-                        <c15:formulaRef>
-                          <c15:sqref>('Graph Data'!$B$3,'Graph Data'!$B$14)</c15:sqref>
-                        </c15:formulaRef>
-                      </c:ext>
-                    </c:extLst>
-                    <c:numCache>
-                      <c:formatCode>0</c:formatCode>
-                      <c:ptCount val="2"/>
-                      <c:pt idx="0">
-                        <c:v>94.498000000000005</c:v>
-                      </c:pt>
-                      <c:pt idx="1">
-                        <c:v>318.06299999999999</c:v>
-                      </c:pt>
-                    </c:numCache>
-                  </c:numRef>
-                </c:xVal>
                 <c:yVal>
-                  <c:numRef>
-                    <c:extLst>
-                      <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
-                        <c15:formulaRef>
-                          <c15:sqref>('Graph Data'!$K$3,'Graph Data'!$K$14)</c15:sqref>
-                        </c15:formulaRef>
-                      </c:ext>
-                    </c:extLst>
-                    <c:numCache>
-                      <c:formatCode>0.0</c:formatCode>
-                      <c:ptCount val="2"/>
-                      <c:pt idx="0">
-                        <c:v>86.834999999999994</c:v>
-                      </c:pt>
-                      <c:pt idx="1">
-                        <c:v>92.555000000000007</c:v>
-                      </c:pt>
-                    </c:numCache>
-                  </c:numRef>
+                  <c:numLit>
+                    <c:formatCode>General</c:formatCode>
+                    <c:ptCount val="1"/>
+                    <c:pt idx="0">
+                      <c:v>1</c:v>
+                    </c:pt>
+                  </c:numLit>
                 </c:yVal>
                 <c:smooth val="0"/>
                 <c:extLst>
                   <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                    <c16:uniqueId val="{00000000-FADB-4C93-A067-1456C06C53AF}"/>
+                    <c16:uniqueId val="{00000000-A164-4DA6-AD07-82E406823E2D}"/>
                   </c:ext>
                 </c:extLst>
               </c15:ser>
@@ -12663,7 +12701,7 @@
                 <c:idx val="3"/>
                 <c:order val="2"/>
                 <c:tx>
-                  <c:v> c. %H (*) L*H %</c:v>
+                  <c:v> b. % H* L*!H L*H %</c:v>
                 </c:tx>
                 <c:spPr>
                   <a:ln w="38100">
@@ -12721,73 +12759,6 @@
                 <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                   <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                     <c16:uniqueId val="{00000002-FADB-4C93-A067-1456C06C53AF}"/>
-                  </c:ext>
-                </c:extLst>
-              </c15:ser>
-            </c15:filteredScatterSeries>
-            <c15:filteredScatterSeries>
-              <c15:ser>
-                <c:idx val="0"/>
-                <c:order val="3"/>
-                <c:tx>
-                  <c:v> d. % H* (*) L*H %</c:v>
-                </c:tx>
-                <c:spPr>
-                  <a:ln w="38100">
-                    <a:solidFill>
-                      <a:srgbClr val="B5B0F3"/>
-                    </a:solidFill>
-                  </a:ln>
-                </c:spPr>
-                <c:marker>
-                  <c:symbol val="none"/>
-                </c:marker>
-                <c:xVal>
-                  <c:numRef>
-                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
-                      <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
-                        <c15:formulaRef>
-                          <c15:sqref>('Graph Data'!$B$6,'Graph Data'!$B$17)</c15:sqref>
-                        </c15:formulaRef>
-                      </c:ext>
-                    </c:extLst>
-                    <c:numCache>
-                      <c:formatCode>0</c:formatCode>
-                      <c:ptCount val="2"/>
-                      <c:pt idx="0">
-                        <c:v>79.626999999999995</c:v>
-                      </c:pt>
-                      <c:pt idx="1">
-                        <c:v>303.755</c:v>
-                      </c:pt>
-                    </c:numCache>
-                  </c:numRef>
-                </c:xVal>
-                <c:yVal>
-                  <c:numRef>
-                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
-                      <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
-                        <c15:formulaRef>
-                          <c15:sqref>('Graph Data'!$K$6,'Graph Data'!$K$17)</c15:sqref>
-                        </c15:formulaRef>
-                      </c:ext>
-                    </c:extLst>
-                    <c:numCache>
-                      <c:formatCode>0.0</c:formatCode>
-                      <c:ptCount val="2"/>
-                      <c:pt idx="0">
-                        <c:v>87.183000000000007</c:v>
-                      </c:pt>
-                      <c:pt idx="1">
-                        <c:v>94.043000000000006</c:v>
-                      </c:pt>
-                    </c:numCache>
-                  </c:numRef>
-                </c:yVal>
-                <c:smooth val="0"/>
-                <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
-                  <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                    <c16:uniqueId val="{00000003-FADB-4C93-A067-1456C06C53AF}"/>
                   </c:ext>
                 </c:extLst>
               </c15:ser>
@@ -12982,7 +12953,7 @@
           <c:x val="0.66137719198143707"/>
           <c:y val="0.24909829825297367"/>
           <c:w val="0.27489919738293583"/>
-          <c:h val="0.16143492169609111"/>
+          <c:h val="0.28779715731326672"/>
         </c:manualLayout>
       </c:layout>
       <c:overlay val="1"/>
@@ -42168,6 +42139,12 @@
     <row r="112" ht="13.2" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="13">
+    <mergeCell ref="V4:AD4"/>
+    <mergeCell ref="AE4:AM4"/>
+    <mergeCell ref="AN4:AV4"/>
+    <mergeCell ref="AW4:BE4"/>
+    <mergeCell ref="A1:L1"/>
+    <mergeCell ref="B4:L4"/>
     <mergeCell ref="B30:L30"/>
     <mergeCell ref="B44:L44"/>
     <mergeCell ref="B57:L57"/>
@@ -42175,12 +42152,6 @@
     <mergeCell ref="M4:U4"/>
     <mergeCell ref="A41:L41"/>
     <mergeCell ref="B17:L17"/>
-    <mergeCell ref="V4:AD4"/>
-    <mergeCell ref="AE4:AM4"/>
-    <mergeCell ref="AN4:AV4"/>
-    <mergeCell ref="AW4:BE4"/>
-    <mergeCell ref="A1:L1"/>
-    <mergeCell ref="B4:L4"/>
   </mergeCells>
   <conditionalFormatting sqref="J14:K15 BC14:BD15 AT14:AU15 AK14:AL15 AB14:AC15 S14:T15 S6:T8 AB6:AC8 AK6:AL8 AT6:AU8 BC6:BD8 J6:K8 J10:K12 BC10:BD12 AT10:AU12 AK10:AL12 AB10:AC12 S10:T12">
     <cfRule type="cellIs" dxfId="236" priority="132" stopIfTrue="1" operator="lessThan">
@@ -46173,8 +46144,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F5919AE2-0160-41E7-B7DF-2FBBFC2636AC}">
   <dimension ref="K17:L25"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I3" sqref="I3"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="I9" sqref="I9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>